<commit_message>
gata labuuuuu, build & run
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23902"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23911"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBA80811-105D-43F7-B28B-BFBB854D5CB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{513EC36E-36E0-4B8D-9C10-7895A0938BA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="156" windowWidth="14160" windowHeight="8268" tabRatio="650" firstSheet="3" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="156" windowWidth="14160" windowHeight="8268" tabRatio="650" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="99">
   <si>
     <t>do not print this form</t>
   </si>
@@ -121,7 +121,7 @@
     <t>R06</t>
   </si>
   <si>
-    <t>Functionalitatea de repetitie e ambigua si nu se intelege exact comportamentul dorit. Nu este justificata existenta campului de activ/inactiv</t>
+    <t>Functionalitatea de repetitie e ambigua si nu se intelege exact comportamentul dorit.</t>
   </si>
   <si>
     <t>R01</t>
@@ -160,7 +160,25 @@
     <t>A01/A02</t>
   </si>
   <si>
-    <t>Nu exista impartire pe layere</t>
+    <t>Nu este mentionata impartirea pe layere in diagrama</t>
+  </si>
+  <si>
+    <t>A04/A02</t>
+  </si>
+  <si>
+    <t>Functiile formTimeUnit, parseFromStringToSeconds ar trebui puse in DateService (poate doar getIntervalInHours sa ramana) si DateService sa se numeasca DateTimeService (data, minute , ore unitati temporale)</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>nu se specifica strategia de error handling. beneficiarul se bazeaza doar pe happy-flow, fara situatii exceptionale</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>Nu s-au folosit interfete.</t>
   </si>
   <si>
     <t>A07</t>
@@ -172,25 +190,10 @@
     <t>Clasa controller nu reflecta rolul ei.</t>
   </si>
   <si>
-    <t>A05</t>
-  </si>
-  <si>
-    <t>nu se specifica strategia de error handling. beneficiarul se bazeaza doar pe happy-flow, fara situatii exceptionale</t>
-  </si>
-  <si>
-    <t>A06</t>
-  </si>
-  <si>
-    <t>Nu s-au folosit interfete.</t>
-  </si>
-  <si>
-    <t>A04</t>
-  </si>
-  <si>
-    <t>Controllers-service</t>
-  </si>
-  <si>
-    <t>Operatiile se efectueaza direct in controller</t>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>Clasele nu au descriere</t>
   </si>
   <si>
     <t>Review Form. Coding Defects</t>
@@ -202,6 +205,54 @@
     <t>Popescu Ionel</t>
   </si>
   <si>
+    <t>C02</t>
+  </si>
+  <si>
+    <t>NewEditController, switchRepeatedCheckbox()</t>
+  </si>
+  <si>
+    <t>else if redundant se poate reduce(127-132) la hideRepeatedTaskModule(!source.isSelected());</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>TaskIO, getTaskFromString()</t>
+  </si>
+  <si>
+    <t>variabila startTime poate fi extrasa din blocul conditional(147-155)</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>TaskIO, read(),51</t>
+  </si>
+  <si>
+    <t>Variabila titleLength nu este folosita</t>
+  </si>
+  <si>
+    <t>C01/C09</t>
+  </si>
+  <si>
+    <t>ArrayTaskList, add(),</t>
+  </si>
+  <si>
+    <t>nu poti accesa o metoda pe un obiect null ca sa verific daca e null</t>
+  </si>
+  <si>
+    <t>C09</t>
+  </si>
+  <si>
+    <t>DefaultTaskService,  filterTask()</t>
+  </si>
+  <si>
+    <t>variabile locale inutile. return direct</t>
+  </si>
+  <si>
+    <t>DefaultDateTimeService, parseFromStringToSeconds()</t>
+  </si>
+  <si>
     <t>Tool-based Code Analysis</t>
   </si>
   <si>
@@ -218,6 +269,84 @@
   </si>
   <si>
     <t>After/Argument</t>
+  </si>
+  <si>
+    <t>NewEditController
+ -&gt; 
+setCurrentTask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"switch" statements should have "default" clauses
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swith (clickedButton.getId()){
+    case "btnNew" : initNewWindow("New Task");
+        break;
+    case "btnEdit" : initEditWindow("Edit Task");
+        break;
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">switch (clickedButton.getId()){
+    case "btnNew" : initNewWindow("New Task");
+        break;
+    case "btnEdit" : initEditWindow("Edit Task");
+        break;
+    default:
+        break;
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NewEditController -&gt; initialize
+</t>
+  </si>
+  <si>
+    <t>Sections of code should not be commented out</t>
+  </si>
+  <si>
+    <t>//        switch (clickedButton.getId()){
+//            case  "btnNew" : initNewWindow("New Task");
+//                break;
+//            case "btnEdit" : initEditWindow("Edit Task");
+//                break;
+//        }</t>
+  </si>
+  <si>
+    <t>NewEditController -&gt; initEditWindow</t>
+  </si>
+  <si>
+    <t>"static" members should be accessed statically</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datePickerStart.setValue(dateService.getLocalDateValueFromDate(currentTask.getStartTime()));datePickerEnd.setValue(dateService.getLocalDateValueFromDate(currentTask.getEndTime()));
+</t>
+  </si>
+  <si>
+    <t>datePickerStart.setValue(DefaultDateTimeService.getLocalDateValueFromDate(currentTask.getStartTime()));datePickerEnd.setValue(DefaultDateTimeService.getLocalDateValueFromDate(currentTask.getEndTime()));</t>
+  </si>
+  <si>
+    <t>NewEditController - &gt; makeTask</t>
+  </si>
+  <si>
+    <t>Standard outputs should not be used directly to log anything</t>
+  </si>
+  <si>
+    <t>System.out.println(result);</t>
+  </si>
+  <si>
+    <t>TaskIO</t>
+  </si>
+  <si>
+    <t>Constant names should comply with a naming convention</t>
+  </si>
+  <si>
+    <t>secondsInMin secondsInHour,secondsInDay</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SECONDS_IN_MIN,SECONDS_IN_HOUR,SECONDS_IN_DAY</t>
   </si>
   <si>
     <t>Effort to perform tool-based code analysis (hours):</t>
@@ -227,7 +356,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,8 +427,32 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,8 +477,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -394,11 +553,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -422,60 +637,103 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -819,8 +1077,8 @@
   </sheetPr>
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -841,27 +1099,27 @@
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="33"/>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="16"/>
       <c r="I2" s="16" t="s">
         <v>3</v>
@@ -871,13 +1129,13 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="16" t="s">
         <v>5</v>
       </c>
@@ -889,17 +1147,17 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="16" t="s">
         <v>10</v>
       </c>
@@ -911,17 +1169,17 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
       <c r="H5" s="16" t="s">
         <v>15</v>
       </c>
@@ -933,37 +1191,37 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="33"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="31">
         <v>44262</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="33"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="9" t="s">
         <v>19</v>
       </c>
@@ -976,14 +1234,14 @@
       <c r="E9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
     </row>
     <row r="10" spans="1:10" ht="30">
-      <c r="A10" s="33"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="16">
         <v>1</v>
       </c>
@@ -996,14 +1254,14 @@
       <c r="E10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
     </row>
     <row r="11" spans="1:10" ht="45">
-      <c r="A11" s="33"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="16">
         <f>B10+1</f>
         <v>2</v>
@@ -1017,14 +1275,14 @@
       <c r="E11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-    </row>
-    <row r="12" spans="1:10" ht="60">
-      <c r="A12" s="33"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" spans="1:10" ht="30">
+      <c r="A12" s="19"/>
       <c r="B12" s="16">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -1035,17 +1293,17 @@
       <c r="D12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
     </row>
     <row r="13" spans="1:10" ht="30">
-      <c r="A13" s="33"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="16">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1059,14 +1317,14 @@
       <c r="E13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
     </row>
     <row r="14" spans="1:10" ht="30">
-      <c r="A14" s="33"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="16">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1080,14 +1338,14 @@
       <c r="E14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="33"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="16">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1095,14 +1353,14 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="16">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1110,11 +1368,11 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="16">
@@ -1132,7 +1390,7 @@
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
-      <c r="E18" s="35"/>
+      <c r="E18" s="20"/>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="16">
@@ -1141,7 +1399,7 @@
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
-      <c r="E19" s="35"/>
+      <c r="E19" s="20"/>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="16">
@@ -1150,7 +1408,7 @@
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
-      <c r="E20" s="35"/>
+      <c r="E20" s="20"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="16">
@@ -1159,7 +1417,7 @@
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="E21" s="35"/>
+      <c r="E21" s="20"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="16">
@@ -1168,7 +1426,7 @@
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
-      <c r="E22" s="35"/>
+      <c r="E22" s="20"/>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="16">
@@ -1177,7 +1435,7 @@
       </c>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="35"/>
+      <c r="E23" s="20"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="16">
@@ -1186,7 +1444,7 @@
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="35"/>
+      <c r="E24" s="20"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="16">
@@ -1195,26 +1453,26 @@
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="35"/>
+      <c r="E25" s="20"/>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="36"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="21"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="33"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="10" t="s">
         <v>36</v>
       </c>
       <c r="D27" s="11"/>
-      <c r="E27" s="32">
+      <c r="E27" s="18">
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="19" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1237,10 +1495,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -1260,27 +1518,27 @@
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="1:10" ht="14.45" customHeight="1">
-      <c r="A2" s="33"/>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="16"/>
       <c r="I2" s="16" t="s">
         <v>3</v>
@@ -1290,13 +1548,13 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.45" customHeight="1">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="16" t="s">
         <v>5</v>
       </c>
@@ -1308,17 +1566,17 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="14.45" customHeight="1">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="16" t="s">
         <v>10</v>
       </c>
@@ -1330,17 +1588,17 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.45" customHeight="1">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
       <c r="H5" s="16" t="s">
         <v>15</v>
       </c>
@@ -1352,37 +1610,37 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15">
-      <c r="A6" s="33"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="31">
         <v>44262</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="33"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+    </row>
+    <row r="9" spans="1:10" ht="15">
+      <c r="A9" s="19"/>
       <c r="B9" s="9" t="s">
         <v>19</v>
       </c>
@@ -1395,14 +1653,14 @@
       <c r="E9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
     </row>
     <row r="10" spans="1:10" ht="30">
-      <c r="A10" s="33"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="16">
         <v>1</v>
       </c>
@@ -1415,14 +1673,14 @@
       <c r="E10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-    </row>
-    <row r="11" spans="1:10" ht="15">
-      <c r="A11" s="33"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+    </row>
+    <row r="11" spans="1:10" ht="75">
+      <c r="A11" s="19"/>
       <c r="B11" s="16">
         <f>B10+1</f>
         <v>2</v>
@@ -1430,94 +1688,104 @@
       <c r="C11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-    </row>
-    <row r="12" spans="1:10" ht="45">
-      <c r="A12" s="33"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" spans="1:10" ht="51.75" customHeight="1">
+      <c r="A12" s="19"/>
       <c r="B12" s="16">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13" spans="1:10" ht="36" customHeight="1">
+      <c r="A13" s="19"/>
+      <c r="B13" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-    </row>
-    <row r="13" spans="1:10" ht="15">
-      <c r="A13" s="33"/>
-      <c r="B13" s="16">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+    </row>
+    <row r="14" spans="1:10" ht="36" customHeight="1">
+      <c r="A14" s="19"/>
+      <c r="B14" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-    </row>
-    <row r="14" spans="1:10" ht="30">
-      <c r="A14" s="33"/>
-      <c r="B14" s="16">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="1:10" ht="44.25" customHeight="1">
+      <c r="A15" s="19"/>
+      <c r="B15" s="16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C15" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-    </row>
-    <row r="15" spans="1:10" ht="15">
-      <c r="A15" s="33"/>
-      <c r="B15" s="16">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
+      <c r="D15" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:10" ht="15">
-      <c r="A16" s="33"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="16">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1525,13 +1793,14 @@
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-    </row>
-    <row r="17" spans="2:5">
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="19"/>
       <c r="B17" s="16">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1539,8 +1808,14 @@
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5">
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="19"/>
       <c r="B18" s="16">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1548,8 +1823,14 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5">
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="19"/>
       <c r="B19" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1557,8 +1838,14 @@
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="2:5">
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="19"/>
       <c r="B20" s="16">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1566,8 +1853,14 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="2:5">
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="19"/>
       <c r="B21" s="16">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1575,8 +1868,14 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="2:5">
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="19"/>
       <c r="B22" s="16">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1584,8 +1883,14 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="2:5">
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="19"/>
       <c r="B23" s="16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1593,8 +1898,14 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="2:5">
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="19"/>
       <c r="B24" s="16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1602,8 +1913,14 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="2:5">
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="19"/>
       <c r="B25" s="16">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1611,8 +1928,14 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="2:5">
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="19"/>
       <c r="B26" s="16">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1620,22 +1943,66 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="2:5">
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="36"/>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="33"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+    </row>
+    <row r="28" spans="1:10" ht="15">
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="10" t="s">
         <v>36</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="1"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+    </row>
+    <row r="29" spans="1:10" ht="15">
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+    </row>
+    <row r="30" spans="1:10" ht="15">
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C10:E15">
+    <sortCondition ref="C10:C15"/>
+  </sortState>
   <mergeCells count="6">
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B2:E2"/>
@@ -1654,10 +2021,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J5"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -1665,7 +2032,7 @@
     <col min="1" max="1" width="8.85546875" style="5"/>
     <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="18" style="5" customWidth="1"/>
+    <col min="4" max="4" width="27" style="5" customWidth="1"/>
     <col min="5" max="5" width="41.42578125" style="5" customWidth="1"/>
     <col min="6" max="8" width="8.85546875" style="5"/>
     <col min="9" max="9" width="26.7109375" style="5" customWidth="1"/>
@@ -1677,27 +2044,27 @@
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="1:10" ht="14.45" customHeight="1">
-      <c r="A2" s="33"/>
-      <c r="B2" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="16"/>
       <c r="I2" s="16" t="s">
         <v>3</v>
@@ -1707,13 +2074,13 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.45" customHeight="1">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="16" t="s">
         <v>5</v>
       </c>
@@ -1725,17 +2092,17 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="14.45" customHeight="1">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="D4" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="47"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="16" t="s">
         <v>10</v>
       </c>
@@ -1747,17 +2114,17 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.45" customHeight="1">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="D5" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="49"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
       <c r="H5" s="16" t="s">
         <v>15</v>
       </c>
@@ -1769,35 +2136,35 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15">
-      <c r="A6" s="33"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="33"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="9" t="s">
         <v>19</v>
       </c>
@@ -1810,258 +2177,248 @@
       <c r="E9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="33"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+    </row>
+    <row r="10" spans="1:10" ht="45">
+      <c r="A10" s="19"/>
       <c r="B10" s="16">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="33"/>
+      <c r="C10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+    </row>
+    <row r="11" spans="1:10" ht="54" customHeight="1">
+      <c r="A11" s="19"/>
       <c r="B11" s="16">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="33"/>
+      <c r="C11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" spans="1:10" ht="15">
+      <c r="A12" s="19"/>
       <c r="B12" s="16">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="33"/>
+      <c r="C12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13" spans="1:10" ht="30">
+      <c r="A13" s="19"/>
       <c r="B13" s="16">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="33"/>
-      <c r="B14" s="16">
+      <c r="C13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+    </row>
+    <row r="14" spans="1:10" ht="30">
+      <c r="A14" s="19"/>
+      <c r="B14" s="43">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="33"/>
-      <c r="B15" s="16">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="33"/>
-      <c r="B16" s="16">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
+      <c r="C14" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="1:10" ht="30">
+      <c r="A15" s="19"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="42"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+    </row>
+    <row r="16" spans="1:10" ht="15">
+      <c r="A16" s="19"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="16">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B17" s="16"/>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="16">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
+    <row r="18" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B18" s="16"/>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="16">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
+    <row r="19" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B19" s="16"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="16">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
+    <row r="20" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B20" s="16"/>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="16">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
+    <row r="21" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B21" s="16"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="16">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
+    <row r="22" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B22" s="16"/>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="16">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
+    <row r="23" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B23" s="16"/>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="16">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
+    <row r="24" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B24" s="16"/>
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="16">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
+    <row r="25" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B25" s="16"/>
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5">
-      <c r="B26" s="16">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
+    <row r="26" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B26" s="16"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5">
-      <c r="B27" s="16">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
+    <row r="27" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B27" s="16"/>
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="16">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
+      <c r="B28" s="16"/>
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="16">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
+      <c r="B29" s="16"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="16">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
+      <c r="B30" s="16"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="36"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="21"/>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="33"/>
+      <c r="B32" s="19"/>
       <c r="C32" s="10" t="s">
         <v>36</v>
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="1"/>
     </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="D4:E4"/>
@@ -2081,18 +2438,18 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="5"/>
     <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="18" style="5" customWidth="1"/>
-    <col min="5" max="5" width="24" style="5" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="95.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="92.28515625" style="5" customWidth="1"/>
     <col min="7" max="8" width="8.85546875" style="5"/>
     <col min="9" max="9" width="26.7109375" style="5" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="5"/>
@@ -2103,27 +2460,27 @@
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="1:10" ht="14.45" customHeight="1">
-      <c r="A2" s="33"/>
-      <c r="B2" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="16"/>
       <c r="I2" s="16" t="s">
         <v>3</v>
@@ -2133,13 +2490,13 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.45" customHeight="1">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="16" t="s">
         <v>5</v>
       </c>
@@ -2151,15 +2508,15 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="14.45" customHeight="1">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+        <v>75</v>
+      </c>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="16" t="s">
         <v>10</v>
       </c>
@@ -2171,15 +2528,15 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.45" customHeight="1">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
       <c r="H5" s="16" t="s">
         <v>15</v>
       </c>
@@ -2191,144 +2548,180 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15">
-      <c r="A6" s="33"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="33"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="33"/>
+        <v>79</v>
+      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+    </row>
+    <row r="10" spans="1:10" ht="135" customHeight="1">
+      <c r="A10" s="19"/>
       <c r="B10" s="16">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="33"/>
+      <c r="C10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+    </row>
+    <row r="11" spans="1:10" ht="89.25" customHeight="1">
+      <c r="A11" s="19"/>
       <c r="B11" s="16">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="33"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" spans="1:10" ht="42.75" customHeight="1">
+      <c r="A12" s="19"/>
       <c r="B12" s="16">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="33"/>
+      <c r="C12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13" spans="1:10" ht="30">
+      <c r="A13" s="19"/>
       <c r="B13" s="16">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="33"/>
+      <c r="C13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+    </row>
+    <row r="14" spans="1:10" ht="30">
+      <c r="A14" s="19"/>
       <c r="B14" s="16">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="33"/>
+      <c r="C14" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="1:10" ht="16.5">
+      <c r="A15" s="19"/>
       <c r="B15" s="16">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="33"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+    </row>
+    <row r="16" spans="1:10" ht="16.5">
+      <c r="A16" s="19"/>
       <c r="B16" s="16">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
+      <c r="D16" s="30"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="16">
@@ -2471,19 +2864,19 @@
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="2:6">
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="33"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="19"/>
     </row>
     <row r="32" spans="2:6">
-      <c r="B32" s="33"/>
-      <c r="C32" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
       <c r="F32" s="15"/>
     </row>
   </sheetData>

</xml_diff>